<commit_message>
VALID INVALID & CRUD done on Current Availability on 29MAY2025
</commit_message>
<xml_diff>
--- a/Utility/CurrentAvailability.xlsx
+++ b/Utility/CurrentAvailability.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sevvelkaranpalanivetrivel/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DC882D-0595-9248-80D8-BF454A4E1ADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EAAE1DB-71E2-FD48-943B-9CB4EB4F2262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16220" xr2:uid="{E51668DC-9EB4-DE4E-BA21-642832947ECA}"/>
   </bookViews>
@@ -35,16 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t xml:space="preserve">Automation </t>
-  </si>
-  <si>
-    <t>A1</t>
-  </si>
-  <si>
-    <t>Will help in in improving the skills</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>${resources}</t>
   </si>
@@ -62,16 +53,88 @@
   </si>
   <si>
     <t>${skill}</t>
+  </si>
+  <si>
+    <t>Fullstack</t>
+  </si>
+  <si>
+    <t>6 Months</t>
+  </si>
+  <si>
+    <t>Batch A</t>
+  </si>
+  <si>
+    <t>Ready to deploy</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>3 Months</t>
+  </si>
+  <si>
+    <t>Batch B</t>
+  </si>
+  <si>
+    <t>Missing resources</t>
+  </si>
+  <si>
+    <t>valid</t>
+  </si>
+  <si>
+    <t>invalid</t>
+  </si>
+  <si>
+    <t>React</t>
+  </si>
+  <si>
+    <t>Batch C</t>
+  </si>
+  <si>
+    <t>Missing duration</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>4 Months</t>
+  </si>
+  <si>
+    <t>No batch specified</t>
+  </si>
+  <si>
+    <t>${type}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -97,8 +160,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94FCC4C6-1347-3D44-98CD-DB111ED93325}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -424,47 +489,117 @@
     <col min="6" max="6" width="28.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E2" s="2">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="2">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="F3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="2">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
+      <c r="F4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>5</v>
-      </c>
-      <c r="C2">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="2">
         <v>1</v>
       </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2">
         <v>2</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>